<commit_message>
ABBIAMO PERSO TEMPO CERCANDO DI INTERPOLARE UNA RETTA CON PARAMETRI ENTRAMBI 0, REALIZZIAMO CHE BASTA FARE MEDIA E DEVIAZONE STANDARD
</commit_message>
<xml_diff>
--- a/PENDOLO DI TORSIONE/dati_pendolo_di_torsione.xlsx
+++ b/PENDOLO DI TORSIONE/dati_pendolo_di_torsione.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="disco rigido" sheetId="1" state="visible" r:id="rId1"/>
@@ -201,14 +201,13 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="3" xfId="0" applyNumberFormat="1"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -779,7 +778,7 @@
       <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3"/>
@@ -795,31 +794,31 @@
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>2630</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>7</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>3590</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>4</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>4190</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>9</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>50</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>70</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>85</v>
       </c>
       <c r="J2" s="3"/>
@@ -828,27 +827,27 @@
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
       <c r="O2" s="3"/>
-      <c r="P2" s="6">
+      <c r="P2" s="5">
         <v>1</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>2570</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>4</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>3600</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>4130</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>15</v>
       </c>
       <c r="G3" s="2"/>
@@ -863,22 +862,22 @@
       <c r="P3" s="2"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>2600</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>3600</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>7</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>4250</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>13</v>
       </c>
       <c r="G4" s="2"/>
@@ -893,22 +892,22 @@
       <c r="P4" s="2"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>2590</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>6</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>3500</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>4</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>4280</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>9</v>
       </c>
       <c r="G5" s="2"/>
@@ -923,22 +922,22 @@
       <c r="P5" s="2"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>2600</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>6</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>3490</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>7</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>4180</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>5</v>
       </c>
       <c r="G6" s="2"/>
@@ -1012,51 +1011,51 @@
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1070</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="4">
         <v>1510</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>2</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>1860</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>5</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>50</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>70</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>85</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" s="5">
+      <c r="A3" s="4">
         <v>1050</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>3</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="4">
         <v>1550</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="4">
         <v>3</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="4">
         <v>1840</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>5</v>
       </c>
       <c r="G3" s="2"/>
@@ -1064,22 +1063,22 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>1080</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="4">
         <v>1540</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="4">
         <v>4</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="4">
         <v>1860</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>4</v>
       </c>
       <c r="G4" s="2"/>
@@ -1087,22 +1086,22 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>1050</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>2</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="4">
         <v>1530</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>2</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="4">
         <v>1850</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>2</v>
       </c>
       <c r="G5" s="2"/>
@@ -1110,22 +1109,22 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>1070</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>1550</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>4</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="4">
         <v>1830</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>4</v>
       </c>
       <c r="G6" s="2"/>
@@ -1153,32 +1152,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" customWidth="1" min="1" max="1" style="7" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="2" max="2" style="7" width="10.290714285714287"/>
-    <col bestFit="1" customWidth="1" min="3" max="3" style="7" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="4" max="4" style="7" width="10.290714285714287"/>
-    <col bestFit="1" customWidth="1" min="5" max="5" style="7" width="12.43357142857143"/>
-    <col bestFit="1" customWidth="1" min="6" max="6" style="7" width="10.290714285714287"/>
+    <col bestFit="1" customWidth="1" min="1" max="1" style="6" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="2" max="2" style="6" width="10.290714285714287"/>
+    <col bestFit="1" customWidth="1" min="3" max="3" style="6" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="4" max="4" style="6" width="10.290714285714287"/>
+    <col bestFit="1" customWidth="1" min="5" max="5" style="6" width="12.43357142857143"/>
+    <col bestFit="1" customWidth="1" min="6" max="6" style="6" width="10.290714285714287"/>
     <col bestFit="1" customWidth="1" min="7" max="9" style="2" width="12.43357142857143"/>
   </cols>
   <sheetData>
     <row r="1" ht="17.25" customHeight="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -1192,51 +1191,51 @@
       </c>
     </row>
     <row r="2" ht="17.25" customHeight="1">
-      <c r="A2" s="8">
+      <c r="A2" s="7">
         <v>74.799999999999997</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="7">
         <v>0.40000000000000002</v>
       </c>
-      <c r="C2" s="8">
+      <c r="C2" s="7">
         <v>97.900000000000006</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>0.29999999999999999</v>
       </c>
-      <c r="E2" s="8">
+      <c r="E2" s="7">
         <v>121</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2" s="7">
         <v>0.29999999999999999</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>50</v>
       </c>
-      <c r="H2" s="6">
+      <c r="H2" s="5">
         <v>70</v>
       </c>
-      <c r="I2" s="6">
+      <c r="I2" s="5">
         <v>85</v>
       </c>
     </row>
     <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>69.099999999999994</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>0.20000000000000001</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>98.700000000000003</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="7">
         <v>0.29999999999999999</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="7">
         <v>120</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>0.40000000000000002</v>
       </c>
       <c r="G3" s="2"/>
@@ -1244,22 +1243,22 @@
       <c r="I3" s="2"/>
     </row>
     <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="8">
+      <c r="A4" s="7">
         <v>68.5</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>0.20000000000000001</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>98.5</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="7">
         <v>0.29999999999999999</v>
       </c>
-      <c r="E4" s="8">
+      <c r="E4" s="7">
         <v>122</v>
       </c>
-      <c r="F4" s="8">
+      <c r="F4" s="7">
         <v>0.29999999999999999</v>
       </c>
       <c r="G4" s="2"/>
@@ -1267,22 +1266,22 @@
       <c r="I4" s="2"/>
     </row>
     <row r="5" ht="17.25" customHeight="1">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>67.200000000000003</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>0.20000000000000001</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>102</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="7">
         <v>0.29999999999999999</v>
       </c>
-      <c r="E5" s="8">
+      <c r="E5" s="7">
         <v>120</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="7">
         <v>0.40000000000000002</v>
       </c>
       <c r="G5" s="2"/>
@@ -1290,22 +1289,22 @@
       <c r="I5" s="2"/>
     </row>
     <row r="6" ht="17.25" customHeight="1">
-      <c r="A6" s="8">
+      <c r="A6" s="7">
         <v>69</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>0.20000000000000001</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>101</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="7">
         <v>0.29999999999999999</v>
       </c>
-      <c r="E6" s="8">
+      <c r="E6" s="7">
         <v>120</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
         <v>0.40000000000000002</v>
       </c>
       <c r="G6" s="2"/>
@@ -1329,7 +1328,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col bestFit="1" min="1" max="1" width="17.8515625"/>
+    <col customWidth="1" min="1" max="1" width="21.7109375"/>
     <col customWidth="1" min="2" max="2" width="12.8515625"/>
     <col bestFit="1" min="3" max="3" width="15.00390625"/>
   </cols>
@@ -1665,7 +1664,7 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>41</v>
       </c>
       <c r="B1" t="s">
@@ -1694,109 +1693,109 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="10">
+      <c r="A2" s="9">
         <v>1.04</v>
       </c>
-      <c r="B2" s="10">
+      <c r="B2" s="9">
         <v>1.04</v>
       </c>
-      <c r="C2" s="10">
+      <c r="C2" s="9">
         <v>1.04</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="9">
         <v>50</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="9">
         <v>250</v>
       </c>
-      <c r="F2" s="10">
+      <c r="F2" s="9">
         <v>550</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="9">
         <v>0.38400000000000001</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="9">
         <v>550</v>
       </c>
-      <c r="I2" s="10">
+      <c r="I2" s="9">
         <v>28.5</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="10">
+      <c r="A3" s="9">
         <v>1.04</v>
       </c>
-      <c r="B3" s="10">
+      <c r="B3" s="9">
         <v>1.04</v>
       </c>
-      <c r="C3" s="10">
+      <c r="C3" s="9">
         <v>1.04</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10">
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9">
         <v>0.55900000000000005</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>750</v>
       </c>
-      <c r="I3" s="10"/>
+      <c r="I3" s="9"/>
     </row>
     <row r="4">
-      <c r="A4" s="10">
+      <c r="A4" s="9">
         <v>1.04</v>
       </c>
-      <c r="B4" s="10">
+      <c r="B4" s="9">
         <v>1.04</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="9">
         <v>1.03</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10">
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9">
         <v>0.69799999999999995</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="9">
         <v>950</v>
       </c>
-      <c r="I4" s="10"/>
+      <c r="I4" s="9"/>
     </row>
     <row r="5">
-      <c r="A5" s="10">
+      <c r="A5" s="9">
         <v>1.03</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="9">
         <v>1.05</v>
       </c>
-      <c r="C5" s="10">
+      <c r="C5" s="9">
         <v>1.04</v>
       </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="9"/>
     </row>
     <row r="6">
-      <c r="A6" s="10">
+      <c r="A6" s="9">
         <v>1.04</v>
       </c>
-      <c r="B6" s="10">
+      <c r="B6" s="9">
         <v>1.03</v>
       </c>
-      <c r="C6" s="10">
+      <c r="C6" s="9">
         <v>1.03</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="0" gridLines="0"/>

</xml_diff>